<commit_message>
Updated Design Fire Creation Kit
- Made changes to the documentation
- Added a UnitTester for Calculating the individuel Phases
- Made the Plotly graph work
- Added the rest of the Phases in the calculator (Steady and Decay)
- Bug in calculating the datapoints for the decay phase.
</commit_message>
<xml_diff>
--- a/Dokumentation/Design Fire Creator/Validation.xlsx
+++ b/Dokumentation/Design Fire Creator/Validation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>y</t>
   </si>
@@ -43,13 +44,51 @@
   <si>
     <t>t_d</t>
   </si>
+  <si>
+    <t>Growth Phase with known Duration and Growth Rate Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration </t>
+  </si>
+  <si>
+    <t>Growth Rate Factor</t>
+  </si>
+  <si>
+    <t>kW/s²</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>Decay Phase with known Duration and Growth Rate Factor</t>
+  </si>
+  <si>
+    <t>InitialYq</t>
+  </si>
+  <si>
+    <t>InitialXt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,11 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3563,16 +3603,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>397422</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>139262</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>515664</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>299198</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>119762</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>417439</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>113193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3859,8 +3899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G4:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4021,10 +4061,7 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="1">
-        <f>0.047*(T6^2-T7^2)+T5</f>
-        <v>1880</v>
-      </c>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L12" s="1">
@@ -4103,10 +4140,7 @@
         <v>380.7</v>
       </c>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1">
-        <f>P17-0.047*(100^2-(100-(100-O17))^2)</f>
-        <v>1880</v>
-      </c>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="12:20" x14ac:dyDescent="0.25">
@@ -5018,4 +5052,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <f>C6*C5^2</f>
+        <v>470</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <f>C15-C18*C17^2</f>
+        <v>530</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bugs in the decay phase calculator
- Changed lib structure in UnitTest for DesignFire
- Created a new UnitTest for Creating DataPoints for Chart
- Fixed the bug in the Decay Phase where incorrent DataPoints were
generated
- Fixed an error in calculating the Total Energy Released in the Decay
Phase.
</commit_message>
<xml_diff>
--- a/Dokumentation/Design Fire Creator/Validation.xlsx
+++ b/Dokumentation/Design Fire Creator/Validation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>y</t>
   </si>
@@ -74,6 +74,27 @@
   <si>
     <t>InitialXt</t>
   </si>
+  <si>
+    <t>One Of Each Phase</t>
+  </si>
+  <si>
+    <t>- Growth Phase with known Duration and Growth Rate Factor</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>StepSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Steady Phase with known Duration </t>
+  </si>
+  <si>
+    <t>- Decay Phase with known Duration and Growth Rate Factor</t>
+  </si>
 </sst>
 </file>
 
@@ -116,12 +137,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,7 +1175,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1267,7 +1292,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1641,7 +1665,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1760,7 +1783,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5056,10 +5078,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D20"/>
+  <dimension ref="B3:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77:F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5158,6 +5180,431 @@
         <v>530</v>
       </c>
     </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <f>C27</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f>C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <f>$C$32*C36</f>
+        <v>10</v>
+      </c>
+      <c r="E36" s="5">
+        <f>$C$31*D36^2</f>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" ref="D37:D45" si="0">$C$32*C37</f>
+        <v>20</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" ref="E37:E45" si="1">$C$31*D37^2</f>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="1"/>
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="1">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="1"/>
+        <v>75.2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="1">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="1"/>
+        <v>117.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="1">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="1"/>
+        <v>169.2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="1"/>
+        <v>230.3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="1"/>
+        <v>300.8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="1"/>
+        <v>380.7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="1">
+        <v>10</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="1"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <f>D45</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="4">
+        <f>E45</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <f>C49</f>
+        <v>100</v>
+      </c>
+      <c r="E55" s="5">
+        <f>C50</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <f>D55+C52</f>
+        <v>200</v>
+      </c>
+      <c r="E56" s="5">
+        <f>E55</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <f>D56</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="4">
+        <f>E56</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>100</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <f>C60</f>
+        <v>200</v>
+      </c>
+      <c r="E67" s="5">
+        <f>C61</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>5</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>6</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="1">
+        <v>9</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C77" s="1">
+        <v>10</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>